<commit_message>
Fixed fixture file- replaced `__interated` by `__last` + fixed typo in a private loop api. (#107)
* Fix typo, changed `insetRows` into `insertRows`. The old version should be removed further.

* Fixed fixture file- replaced `__interated` by `__last` closes https://github.com/Siemienik/XToolset/issues/96

* Added `expected.xlsx` into `ForEach-special` test
</commit_message>
<xml_diff>
--- a/packages/xlsx-renderer/tests/integration/data/Renderer012-ForEach-special/expected.xlsx
+++ b/packages/xlsx-renderer/tests/integration/data/Renderer012-ForEach-special/expected.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27795" windowHeight="16440" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27800" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet sheetId="1" name="Most common for each" state="visible" r:id="rId4"/>
@@ -13,14 +13,13 @@
     <sheet sheetId="3" name="Looping thought ws 3" state="visible" r:id="rId7"/>
     <sheet sheetId="5" name="Looping thought ws 4" state="visible" r:id="rId8"/>
     <sheet sheetId="6" name="Looping thought ws 5" state="visible" r:id="rId9"/>
-    <sheet sheetId="7" name="Looping thought ws 6" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="54">
   <si>
     <t>FOR EACH special item</t>
   </si>
@@ -43,6 +42,9 @@
     <t>__iterated</t>
   </si>
   <si>
+    <t>__last</t>
+  </si>
+  <si>
     <t>__insertRows</t>
   </si>
   <si>
@@ -109,6 +111,9 @@
     <t>`__iterated` - iteration has been finished</t>
   </si>
   <si>
+    <t>`__last` - is this last element of a collection</t>
+  </si>
+  <si>
     <t>`__insetRows` - second and next iterations have to insert new rows</t>
   </si>
   <si>
@@ -118,6 +123,9 @@
     <t>`__endOutput` - last output cell</t>
   </si>
   <si>
+    <t>&lt;- delete item</t>
+  </si>
+  <si>
     <t>KEY</t>
   </si>
   <si>
@@ -125,6 +133,9 @@
   </si>
   <si>
     <t xml:space="preserve"> item.__iterated</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> item.__last</t>
   </si>
   <si>
     <t xml:space="preserve"> item.__insertRows</t>
@@ -375,55 +386,6 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>923925</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>448088</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -769,20 +731,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="Q1" sqref="Q1"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2" defaultColWidth="8.83203125"/>
   <cols>
-    <col min="1" max="10" width="10" customWidth="1"/>
-    <col min="11" max="16" width="13.5703125" customWidth="1"/>
-    <col min="17" max="18" width="10" customWidth="1"/>
+    <col min="1" max="11" width="10" customWidth="1"/>
+    <col min="12" max="17" width="13.5" customWidth="1"/>
+    <col min="18" max="19" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -801,36 +763,38 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q1" s="1"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="G2" s="1"/>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="M2" s="1"/>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="1"/>
+      <c r="O2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="1"/>
       <c r="P2" s="1"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q2" s="1"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -879,28 +843,34 @@
       <c r="P3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="b">
         <v>0</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4">
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4">
         <v>3</v>
       </c>
-      <c r="F4">
-        <v>17</v>
-      </c>
       <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>4</v>
+        <v>18</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
       </c>
       <c r="L4">
         <v>4</v>
@@ -908,37 +878,43 @@
       <c r="M4">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="b">
         <v>0</v>
       </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5">
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5">
         <v>3</v>
       </c>
-      <c r="F5">
-        <v>17</v>
-      </c>
       <c r="G5">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="H5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="K5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L5">
         <v>4</v>
@@ -946,37 +922,43 @@
       <c r="M5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="b">
         <v>0</v>
       </c>
-      <c r="C6">
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6">
         <v>3</v>
       </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6">
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6">
         <v>3</v>
       </c>
-      <c r="F6">
-        <v>17</v>
-      </c>
       <c r="G6">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="H6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="K6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L6">
         <v>4</v>
@@ -984,37 +966,43 @@
       <c r="M6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="b">
         <v>0</v>
       </c>
-      <c r="C7">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7">
+      <c r="B7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7">
         <v>3</v>
       </c>
-      <c r="F7">
-        <v>17</v>
-      </c>
       <c r="G7">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="H7">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="K7">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L7">
         <v>4</v>
@@ -1022,43 +1010,49 @@
       <c r="M7">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" t="b">
+        <v>1</v>
+      </c>
+      <c r="B10" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" t="b">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10">
+      <c r="F10">
         <v>3</v>
       </c>
-      <c r="F10">
-        <v>17</v>
-      </c>
       <c r="G10">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="H10">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I10">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="K10">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L10">
         <v>4</v>
@@ -1067,7 +1061,7 @@
         <v>4</v>
       </c>
       <c r="N10">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="O10">
         <v>7</v>
@@ -1075,63 +1069,70 @@
       <c r="P10">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Q10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="O2:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1139,18 +1140,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q19"/>
+  <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2" defaultColWidth="8.83203125"/>
   <cols>
-    <col min="1" max="16" width="16.5703125" customWidth="1"/>
+    <col min="1" max="17" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1199,28 +1200,34 @@
       <c r="P1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="b">
         <v>0</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
       </c>
       <c r="F2">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>2</v>
+        <v>18</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
       </c>
       <c r="L2">
         <v>2</v>
@@ -1228,37 +1235,43 @@
       <c r="M2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="b">
         <v>0</v>
       </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
       </c>
       <c r="F3">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="H3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="K3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L3">
         <v>2</v>
@@ -1266,37 +1279,43 @@
       <c r="M3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="b">
         <v>0</v>
       </c>
-      <c r="C4">
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
+      <c r="E4" t="s">
+        <v>23</v>
       </c>
       <c r="F4">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="H4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I4">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="K4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L4">
         <v>2</v>
@@ -1304,37 +1323,43 @@
       <c r="M4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="b">
         <v>0</v>
       </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
+      <c r="B5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
       </c>
       <c r="F5">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I5">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="K5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L5">
         <v>2</v>
@@ -1342,11 +1367,18 @@
       <c r="M5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1395,28 +1427,34 @@
       <c r="P9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="b">
         <v>0</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10">
+      <c r="B10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10">
         <v>6</v>
       </c>
-      <c r="F10">
-        <v>17</v>
-      </c>
       <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="K10">
-        <v>10</v>
+        <v>18</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
       </c>
       <c r="L10">
         <v>10</v>
@@ -1424,37 +1462,43 @@
       <c r="M10">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="b">
         <v>0</v>
       </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11">
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11">
         <v>6</v>
       </c>
-      <c r="F11">
-        <v>17</v>
-      </c>
       <c r="G11">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
         <v>7</v>
       </c>
-      <c r="I11">
-        <v>17</v>
-      </c>
       <c r="J11">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="K11">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="L11">
         <v>10</v>
@@ -1462,37 +1506,43 @@
       <c r="M11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="b">
         <v>0</v>
       </c>
-      <c r="C12">
+      <c r="B12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C12" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12">
         <v>3</v>
       </c>
-      <c r="D12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12">
+      <c r="E12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12">
         <v>6</v>
       </c>
-      <c r="F12">
-        <v>17</v>
-      </c>
       <c r="G12">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
         <v>7</v>
       </c>
-      <c r="I12">
-        <v>17</v>
-      </c>
       <c r="J12">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="K12">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="L12">
         <v>10</v>
@@ -1500,37 +1550,43 @@
       <c r="M12">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="b">
         <v>0</v>
       </c>
-      <c r="C13">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13">
+      <c r="B13" t="b">
+        <v>1</v>
+      </c>
+      <c r="C13" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13">
         <v>6</v>
       </c>
-      <c r="F13">
-        <v>17</v>
-      </c>
       <c r="G13">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
         <v>7</v>
       </c>
-      <c r="I13">
-        <v>17</v>
-      </c>
       <c r="J13">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="K13">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="L13">
         <v>10</v>
@@ -1538,13 +1594,16 @@
       <c r="M13">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25"/>
+      <c r="N13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1552,28 +1611,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2" defaultColWidth="8.83203125"/>
   <cols>
-    <col min="1" max="3" width="28.42578125" customWidth="1"/>
+    <col min="1" max="3" width="28.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B2" t="b">
         <v>0</v>
@@ -1581,75 +1640,78 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>38</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
+        <v>39</v>
+      </c>
+      <c r="B4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
+        <v>40</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>44</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -1657,7 +1719,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -1665,26 +1727,34 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>50</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+    </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
@@ -1694,28 +1764,28 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2" defaultColWidth="8.83203125"/>
   <cols>
-    <col min="1" max="3" width="28.42578125" customWidth="1"/>
+    <col min="1" max="3" width="28.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B2" t="b">
         <v>0</v>
@@ -1723,75 +1793,78 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>38</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
+        <v>39</v>
+      </c>
+      <c r="B4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
+        <v>40</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>44</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -1799,7 +1872,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -1807,26 +1880,34 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>50</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+    </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1835,28 +1916,28 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2" defaultColWidth="8.83203125"/>
   <cols>
-    <col min="1" max="3" width="28.42578125" customWidth="1"/>
+    <col min="1" max="3" width="28.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B2" t="b">
         <v>0</v>
@@ -1864,75 +1945,78 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>38</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
+        <v>39</v>
+      </c>
+      <c r="B4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
+        <v>40</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>44</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -1940,7 +2024,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -1948,26 +2032,34 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>50</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+    </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
@@ -1977,28 +2069,28 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2" defaultColWidth="8.83203125"/>
   <cols>
-    <col min="1" max="3" width="28.42578125" customWidth="1"/>
+    <col min="1" max="3" width="28.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B2" t="b">
         <v>0</v>
@@ -2006,75 +2098,78 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>38</v>
+      </c>
+      <c r="B3" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
+        <v>39</v>
+      </c>
+      <c r="B4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
+        <v>40</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>44</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -2082,7 +2177,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -2090,54 +2185,34 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>50</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+    </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="B20" sqref="B20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="28.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" t="s">
-        <v>33</v>
-      </c>
-    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>